<commit_message>
Extracting concept from one phrase
</commit_message>
<xml_diff>
--- a/DATA/Vocabularies/actors.xlsx
+++ b/DATA/Vocabularies/actors.xlsx
@@ -471,13 +471,13 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>['COSATU', ' FOSATU', ' NEHAWU', ' SATAWU', ' Allied', ' AMCU', ' Nuhhrccaw', ' Denosa', ' HOSPERSA', ' NPSWU', ' NUPSAW', ' SADNU', ' POPCRU', ' NASUWU', ' IMATU', ' Union', ' Shop stewart', ' Shop steward', ' Shopsteward', ' Shopstewart', ' Shop-steward', ' Shop-stewart']</t>
+          <t>['COSATU', 'FOSATU', 'NEHAWU', 'SATAWU', 'Allied', 'AMCU', 'Nuhhrccaw', 'Denosa', 'HOSPERSA', 'NPSWU', 'NUPSAW', 'SADNU', 'POPCRU', 'NASUWU', 'IMATU', 'Union', 'Shop stewart', 'Shop steward', 'Shopsteward', 'Shopstewart', 'Shop-steward', 'Shop-stewart']</t>
         </is>
       </c>
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr">
         <is>
-          <t>['cosatu', 'fosatu', 'nehawu', 'satawu', 'ally', 'amcu', 'nuhhrccaw', 'denosa', 'hospersa', 'npswu', 'nupsaw', 'sadnu', 'popcru', 'nasuwu', 'imatu', 'union', 'shop', 'stewart', 'shop', 'steward', 'shopsteward', 'shopstewart', 'shop-steward', 'shop-stewart']</t>
+          <t>['cosatu,fosatu,nehawu,satawu,allied,amcu,nuhhrccaw,denosa,hospersa,npswu,nupsaw,sadnu,popcru,nasuwu,imatu,union,shop', 'stewart,shop', 'steward,shopsteward,shopstewart,shop-steward,shop-stewart']</t>
         </is>
       </c>
       <c r="F2" t="inlineStr"/>
@@ -493,13 +493,13 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>['ANC', ' Congress', ' DA', ' EFF', ' IFP', ' NFP', ' Cope', ' UDM', ' SACP', ' ACDP']</t>
+          <t>['ANC', 'Congress', 'DA', 'EFF', 'IFP', 'NFP', 'Cope', 'UDM', 'SACP', 'ACDP']</t>
         </is>
       </c>
       <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr">
         <is>
-          <t>['anc', 'congress', 'da', 'eff', 'ifp', 'nfp', 'cope', 'udm', 'sacp', 'acdp']</t>
+          <t>['anc,congress,da,eff,ifp,nfp,cope,udm,sacp,acdp']</t>
         </is>
       </c>
       <c r="F3" t="inlineStr"/>
@@ -515,13 +515,13 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>['association', ' residents', ' concerned', ' ratepayers', ' taxpayers', ' NGO', ' organisation', ' ']</t>
+          <t>['association', 'residents', 'concerned', 'ratepayers', 'taxpayers', 'NGO', 'organisation']</t>
         </is>
       </c>
       <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr">
         <is>
-          <t>['association', 'resident', 'concerned', 'ratepayer', 'taxpayer', 'ngo', 'organisation']</t>
+          <t>['association,residents,concerned,ratepayers,taxpayers,ngo,organisation']</t>
         </is>
       </c>
       <c r="F4" t="inlineStr"/>
@@ -537,13 +537,13 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>['church', ' congregation', ' believers', ' temple', ' mosque', ' synagoge']</t>
+          <t>['church', 'congregation', 'believers', 'temple', 'mosque', 'synagoge']</t>
         </is>
       </c>
       <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr">
         <is>
-          <t>['church', 'congregation', 'believer', 'temple', 'mosque', 'synagoge']</t>
+          <t>['church,congregation,believers,temple,mosque,synagoge']</t>
         </is>
       </c>
       <c r="F5" t="inlineStr"/>

</xml_diff>

<commit_message>
Updated Associated Content Analysis Features
</commit_message>
<xml_diff>
--- a/DATA/Vocabularies/actors.xlsx
+++ b/DATA/Vocabularies/actors.xlsx
@@ -462,7 +462,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -484,7 +484,7 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -506,7 +506,7 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -528,7 +528,7 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>

</xml_diff>